<commit_message>
corrected file output directories
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieglinde.hoedl\AI_Mars3D\src_uptodate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieglinde.hoedl\AI_Mars3D\src_uptodate\outputs\MARS_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1029,7 +1029,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1063,8 @@
     <col min="60" max="60" width="10.5703125" style="30" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="46.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="44.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="9.140625" style="30"/>
+    <col min="63" max="63" width="9.140625" style="30" customWidth="1"/>
+    <col min="64" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1846,7 +1847,7 @@
         <v>-15929</v>
       </c>
       <c r="AJ5" s="9">
-        <f t="shared" ref="AJ5:BH5" si="1">AJ4-AJ3</f>
+        <f t="shared" ref="AJ5:BO5" si="1">AJ4-AJ3</f>
         <v>-2291</v>
       </c>
       <c r="AK5" s="8">
@@ -2451,7 +2452,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="9">
-        <f t="shared" ref="AJ8:BH8" si="3">AJ7-AJ6</f>
+        <f t="shared" ref="AJ8:BO8" si="3">AJ7-AJ6</f>
         <v>0</v>
       </c>
       <c r="AK8" s="8">
@@ -3064,7 +3065,7 @@
         <v>-29379</v>
       </c>
       <c r="AJ11" s="9">
-        <f t="shared" ref="AJ11:BH11" si="5">AJ10-AJ9</f>
+        <f t="shared" ref="AJ11:BO11" si="5">AJ10-AJ9</f>
         <v>1010</v>
       </c>
       <c r="AK11" s="8">
@@ -3677,7 +3678,7 @@
         <v>-3588</v>
       </c>
       <c r="AJ14" s="9">
-        <f t="shared" ref="AJ14:BH14" si="7">AJ13-AJ12</f>
+        <f t="shared" ref="AJ14:BO14" si="7">AJ13-AJ12</f>
         <v>0</v>
       </c>
       <c r="AK14" s="8">
@@ -4290,7 +4291,7 @@
         <v>-197</v>
       </c>
       <c r="AJ17" s="9">
-        <f t="shared" ref="AJ17:BH17" si="9">AJ16-AJ15</f>
+        <f t="shared" ref="AJ17:BO17" si="9">AJ16-AJ15</f>
         <v>1029</v>
       </c>
       <c r="AK17" s="8">
@@ -4903,7 +4904,7 @@
         <v>-362</v>
       </c>
       <c r="AJ20" s="13">
-        <f t="shared" ref="AJ20:BH20" si="11">AJ19-AJ18</f>
+        <f t="shared" ref="AJ20:BO20" si="11">AJ19-AJ18</f>
         <v>-425</v>
       </c>
       <c r="AK20" s="12">

</xml_diff>

<commit_message>
added outlier parameter and export of distances with coordinates
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -752,13 +752,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ23"/>
+  <dimension ref="A1:BK29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AV3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="BI13" sqref="BI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -787,13 +787,14 @@
     <col width="12.5703125" bestFit="1" customWidth="1" style="30" min="55" max="55"/>
     <col width="10.28515625" bestFit="1" customWidth="1" style="30" min="56" max="56"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="30" min="57" max="57"/>
-    <col hidden="1" width="20.42578125" customWidth="1" style="30" min="58" max="58"/>
+    <col hidden="1" width="20.7109375" customWidth="1" style="30" min="58" max="58"/>
     <col width="10.28515625" bestFit="1" customWidth="1" style="30" min="59" max="59"/>
     <col width="10.5703125" bestFit="1" customWidth="1" style="30" min="60" max="60"/>
     <col width="46.42578125" bestFit="1" customWidth="1" style="30" min="61" max="61"/>
     <col width="44.5703125" bestFit="1" customWidth="1" style="30" min="62" max="62"/>
-    <col width="9.140625" customWidth="1" style="30" min="63" max="63"/>
-    <col width="9.140625" customWidth="1" style="30" min="64" max="16384"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" style="30" min="63" max="63"/>
+    <col width="9.140625" customWidth="1" style="30" min="64" max="64"/>
+    <col width="9.140625" customWidth="1" style="30" min="65" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="39.75" customHeight="1" s="30">
@@ -1216,6 +1217,11 @@
           <t>Params Path</t>
         </is>
       </c>
+      <c r="BK2" s="1" t="inlineStr">
+        <is>
+          <t>Outlier RMSE Multiplicator</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -1414,6 +1420,7 @@
           <t>data\0342-0349\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK3" s="27" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -1608,6 +1615,7 @@
           <t>data\0342-0349\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK4" s="27" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="n"/>
@@ -1847,6 +1855,7 @@
       </c>
       <c r="BI5" s="25" t="n"/>
       <c r="BJ5" s="10" t="n"/>
+      <c r="BK5" s="10" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -2041,6 +2050,7 @@
           <t>data\0817-0821\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK6" s="27" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -2235,6 +2245,7 @@
           <t>data\0817-0821\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK7" s="27" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n"/>
@@ -2474,6 +2485,7 @@
       </c>
       <c r="BI8" s="7" t="n"/>
       <c r="BJ8" s="28" t="n"/>
+      <c r="BK8" s="28" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -2672,6 +2684,7 @@
           <t>data\0910-0913\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK9" s="27" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -2870,6 +2883,7 @@
           <t>data\0910-0913\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK10" s="27" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -3109,6 +3123,7 @@
       </c>
       <c r="BI11" s="7" t="n"/>
       <c r="BJ11" s="28" t="n"/>
+      <c r="BK11" s="28" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -3307,6 +3322,7 @@
           <t>data\1130-1133\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK12" s="27" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -3505,6 +3521,7 @@
           <t>data\1130-1133\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK13" s="27" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="7" t="n"/>
@@ -3744,6 +3761,7 @@
       </c>
       <c r="BI14" s="7" t="n"/>
       <c r="BJ14" s="28" t="n"/>
+      <c r="BK14" s="28" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
@@ -3942,6 +3960,7 @@
           <t>data\1203-1206\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK15" s="27" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -4140,6 +4159,7 @@
           <t>data\1203-1206\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK16" s="27" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n"/>
@@ -4379,6 +4399,7 @@
       </c>
       <c r="BI17" s="7" t="n"/>
       <c r="BJ17" s="28" t="n"/>
+      <c r="BK17" s="28" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -4577,6 +4598,7 @@
           <t>data\1306-1311\python_ref_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK18" s="27" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -4775,6 +4797,7 @@
           <t>data\1306-1311\python_ref_ai_m3c2_params.txt</t>
         </is>
       </c>
+      <c r="BK19" s="27" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="11" t="n"/>
@@ -5014,6 +5037,7 @@
       </c>
       <c r="BI20" s="11" t="n"/>
       <c r="BJ20" s="29" t="n"/>
+      <c r="BK20" s="29" t="n"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5607,6 +5631,1203 @@
         <is>
           <t>data\0342-0349\python_ref_m3c2_params.txt</t>
         </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-26 12:32:52</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>7092</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.1600419060128736</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3200838120257473</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>7092</v>
+      </c>
+      <c r="K24" t="n">
+        <v>2.839621000000001</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.771547998163</v>
+      </c>
+      <c r="M24" t="n">
+        <v>6930</v>
+      </c>
+      <c r="N24" t="n">
+        <v>-9.280159999999999</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.550929832646</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-0.206625</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.129987</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.002352</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.01580491259097371</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.00793888649182177</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.006524181299999999</v>
+      </c>
+      <c r="X24" t="n">
+        <v>-0.047173</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.047283</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>-0.001339128427128427</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>-0.0024915</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.008916235435993835</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.008815100079166922</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.006200428571428571</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0.006284000099999998</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>6930</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>2492</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>4438</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>155</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>162</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0.07481346296296296</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>0.04401847104960512</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>-0.0119003</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>-0.005849</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>0.002804</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>0.01820599999999998</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>0.008653000000000001</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>-0.01190965</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>-0.0059685</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>0.0025125</v>
+      </c>
+      <c r="AV24" t="n">
+        <v>0.01220904999999999</v>
+      </c>
+      <c r="AW24" t="n">
+        <v>0.008480999999999999</v>
+      </c>
+      <c r="AX24" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="AY24" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="AZ24" t="n">
+        <v>3728747806830.092</v>
+      </c>
+      <c r="BA24" t="n">
+        <v>2.890571413473017</v>
+      </c>
+      <c r="BB24" t="n">
+        <v>0.05758274744334384</v>
+      </c>
+      <c r="BC24" t="n">
+        <v>-0.05171601632923778</v>
+      </c>
+      <c r="BD24" t="n">
+        <v>-0.001999348435514518</v>
+      </c>
+      <c r="BE24" t="n">
+        <v>0.2049253528234164</v>
+      </c>
+      <c r="BF24" t="n">
+        <v>2574637352.242263</v>
+      </c>
+      <c r="BG24" t="n">
+        <v>3.731205478580534</v>
+      </c>
+      <c r="BH24" t="n">
+        <v>28.37070283905381</v>
+      </c>
+      <c r="BI24" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ24" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-26 12:33:19</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>7092</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.1600419060128736</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3200838120257473</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>7092</v>
+      </c>
+      <c r="K25" t="n">
+        <v>2.839621000000001</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1.771547998163</v>
+      </c>
+      <c r="M25" t="n">
+        <v>6988</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-6.452768999999999</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.722783610929</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.206625</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.129987</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-0.002352</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.01580491259097371</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.00793888649182177</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.006524181299999999</v>
+      </c>
+      <c r="X25" t="n">
+        <v>-0.057902</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.062941</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>-0.0009234071265025757</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>-0.002443</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0.01017015800055714</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0.01012815052391209</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0.006599373926731539</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>0.006392971199999999</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>6988</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>2547</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>4441</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>104</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0.08934990384615384</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>0.04583522266615642</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>-0.0119003</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>-0.005849</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>0.002804</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0.01820599999999998</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0.008653000000000001</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>-0.01190995</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>-0.0059435</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>0.00265625</v>
+      </c>
+      <c r="AV25" t="n">
+        <v>0.01361664999999999</v>
+      </c>
+      <c r="AW25" t="n">
+        <v>0.00859975</v>
+      </c>
+      <c r="AX25" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>3728747806830.092</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>2.890571413473017</v>
+      </c>
+      <c r="BB25" t="n">
+        <v>0.05758274744334384</v>
+      </c>
+      <c r="BC25" t="n">
+        <v>-0.05171601632923778</v>
+      </c>
+      <c r="BD25" t="n">
+        <v>-0.001999348435514518</v>
+      </c>
+      <c r="BE25" t="n">
+        <v>0.2049253528234164</v>
+      </c>
+      <c r="BF25" t="n">
+        <v>2574637352.242263</v>
+      </c>
+      <c r="BG25" t="n">
+        <v>3.731205478580534</v>
+      </c>
+      <c r="BH25" t="n">
+        <v>28.37070283905381</v>
+      </c>
+      <c r="BI25" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ25" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-26 12:33:36</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>7092</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.1600419060128736</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3200838120257473</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>7092</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2.839621000000001</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1.771547998163</v>
+      </c>
+      <c r="M26" t="n">
+        <v>7014</v>
+      </c>
+      <c r="N26" t="n">
+        <v>-4.748983999999999</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.856239979132</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-0.206625</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.129987</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-0.002352</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.01580491259097371</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.00793888649182177</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.006524181299999999</v>
+      </c>
+      <c r="X26" t="n">
+        <v>-0.077197</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.078912</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>-0.0006770721414314228</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>-0.002428</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0.01104879384042443</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0.01102802877415081</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0.006839835186769319</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>0.0064307775</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>7014</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>2572</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>4442</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>75</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>78</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>0.09728980769230769</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>0.04763834077609037</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>-0.0119003</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>-0.005849</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>0.002804</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>0.01820599999999998</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>0.008653000000000001</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>-0.01190905</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>-0.0058975</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>0.002689</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>0.01451279999999997</v>
+      </c>
+      <c r="AW26" t="n">
+        <v>0.0085865</v>
+      </c>
+      <c r="AX26" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>3728747806830.092</v>
+      </c>
+      <c r="BA26" t="n">
+        <v>2.890571413473017</v>
+      </c>
+      <c r="BB26" t="n">
+        <v>0.05758274744334384</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>-0.05171601632923778</v>
+      </c>
+      <c r="BD26" t="n">
+        <v>-0.001999348435514518</v>
+      </c>
+      <c r="BE26" t="n">
+        <v>0.2049253528234164</v>
+      </c>
+      <c r="BF26" t="n">
+        <v>2574637352.242263</v>
+      </c>
+      <c r="BG26" t="n">
+        <v>3.731205478580534</v>
+      </c>
+      <c r="BH26" t="n">
+        <v>28.37070283905381</v>
+      </c>
+      <c r="BI26" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ26" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-26 12:36:18</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>7092</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.1600419060128736</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3200838120257473</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>7092</v>
+      </c>
+      <c r="K27" t="n">
+        <v>2.839621000000001</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1.771547998163</v>
+      </c>
+      <c r="M27" t="n">
+        <v>6930</v>
+      </c>
+      <c r="N27" t="n">
+        <v>-9.280159999999999</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.550929832646</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-0.206625</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.129987</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="S27" t="n">
+        <v>-0.002352</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.01580491259097371</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.00793888649182177</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.006524181299999999</v>
+      </c>
+      <c r="X27" t="n">
+        <v>-0.047173</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.047283</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>-0.001339128427128427</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>-0.0024915</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0.008916235435993835</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0.008815100079166922</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0.006200428571428571</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0.006284000099999998</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>6930</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>2492</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>4438</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>155</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>162</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>0.07481346296296296</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>0.04401847104960512</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>-0.0119003</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>-0.005849</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>0.002804</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0.01820599999999998</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0.008653000000000001</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>-0.01190965</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>-0.0059685</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>0.0025125</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>0.01220904999999999</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>0.008480999999999999</v>
+      </c>
+      <c r="AX27" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="AY27" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>3728747806830.092</v>
+      </c>
+      <c r="BA27" t="n">
+        <v>2.890571413473017</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>0.05758274744334384</v>
+      </c>
+      <c r="BC27" t="n">
+        <v>-0.05171601632923778</v>
+      </c>
+      <c r="BD27" t="n">
+        <v>-0.001999348435514518</v>
+      </c>
+      <c r="BE27" t="n">
+        <v>0.2049253528234164</v>
+      </c>
+      <c r="BF27" t="n">
+        <v>2574637352.242263</v>
+      </c>
+      <c r="BG27" t="n">
+        <v>3.731205478580534</v>
+      </c>
+      <c r="BH27" t="n">
+        <v>28.37070283905381</v>
+      </c>
+      <c r="BI27" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ27" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-26 12:56:46</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>7092</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.1600419060128736</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.3200838120257473</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>7092</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2.839621000000001</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.771547998163</v>
+      </c>
+      <c r="M28" t="n">
+        <v>6930</v>
+      </c>
+      <c r="N28" t="n">
+        <v>-9.280159999999999</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.550929832646</v>
+      </c>
+      <c r="P28" t="n">
+        <v>-0.206625</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.129987</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="S28" t="n">
+        <v>-0.002352</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.01580491259097371</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.00793888649182177</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.006524181299999999</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-0.047173</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.047283</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>-0.001339128427128427</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>-0.0024915</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.008916235435993835</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.008815100079166922</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.006200428571428571</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.006284000099999998</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>6930</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>2492</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>4438</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>155</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>162</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>0.07481346296296296</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>0.04401847104960512</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>-0.0119003</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>-0.005849</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>0.002804</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>0.01820599999999998</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>0.008653000000000001</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>-0.01190965</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>-0.0059685</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>0.0025125</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>0.01220904999999999</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>0.008480999999999999</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>0.00040039777213762</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>0.01579983998755641</v>
+      </c>
+      <c r="AZ28" t="n">
+        <v>3728747806830.092</v>
+      </c>
+      <c r="BA28" t="n">
+        <v>2.890571413473017</v>
+      </c>
+      <c r="BB28" t="n">
+        <v>0.05758274744334384</v>
+      </c>
+      <c r="BC28" t="n">
+        <v>-0.05171601632923778</v>
+      </c>
+      <c r="BD28" t="n">
+        <v>-0.001999348435514518</v>
+      </c>
+      <c r="BE28" t="n">
+        <v>0.2049253528234164</v>
+      </c>
+      <c r="BF28" t="n">
+        <v>2574637352.242263</v>
+      </c>
+      <c r="BG28" t="n">
+        <v>3.731205478580534</v>
+      </c>
+      <c r="BH28" t="n">
+        <v>28.37070283905381</v>
+      </c>
+      <c r="BI28" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ28" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-26 13:03:29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G29" t="n">
+        <v>95</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J29" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L29" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M29" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O29" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P29" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X29" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="AX29" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="AZ29" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BA29" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BC29" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BD29" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BE29" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BF29" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BG29" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BH29" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BI29" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ29" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK29" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update only_stats configuration to generate statistics and inlier/outlier files; enhance logging for outlier removal process
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -752,7 +752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK29"/>
+  <dimension ref="A1:BK30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="AV3" activePane="bottomRight" state="frozen"/>
@@ -6830,6 +6830,207 @@
         <v>3</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-26 14:16:15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G30" t="n">
+        <v>95</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J30" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L30" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M30" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N30" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O30" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P30" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R30" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S30" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AW30" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="AX30" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="AY30" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BC30" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BD30" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BE30" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BF30" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BG30" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BH30" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BI30" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ30" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK30" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BB20">
     <sortState ref="A2:BC25">

</xml_diff>

<commit_message>
enhance outlier processing and visualization; add logging for RMS and outlier threshold, implement PLY export for inliers/outliers
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -752,7 +752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK30"/>
+  <dimension ref="A1:BK32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="AV3" activePane="bottomRight" state="frozen"/>
@@ -7031,6 +7031,408 @@
         <v>3</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-26 14:31:24</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G31" t="n">
+        <v>95</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J31" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L31" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M31" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N31" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O31" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R31" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S31" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BB31" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BC31" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BD31" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BE31" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BF31" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BG31" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BH31" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BI31" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ31" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-26 14:36:00</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G32" t="n">
+        <v>95</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J32" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L32" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M32" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N32" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O32" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P32" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R32" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X32" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BC32" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BD32" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BE32" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BF32" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BG32" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BH32" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BI32" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BJ32" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+      <c r="BK32" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BB20">
     <sortState ref="A2:BC25">

</xml_diff>

<commit_message>
Refactor BatchOrchestrator and remove unused strategies
- Removed the ScaleStrategy and VoxelScanStrategy from the BatchOrchestrator.
- Simplified strategy initialization to always use RadiusScanStrategy.
- Enhanced error handling during outlier exclusion and .ply file generation.
- Updated logging messages for clarity.

Clean up strategies.py by removing unused voxel-based strategy code

- Deleted the VoxelScanStrategy and associated helper functions.
- Removed unnecessary comments and code related to voxel partitioning and roughness evaluation.

Improve visualization service error handling

- Added checks for empty TXT files and reshaped arrays if necessary.
- Ensured that the visualization service raises appropriate errors for invalid input data.
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -706,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL21"/>
+  <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -5222,6 +5222,3045 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:29:12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>data\0910-0913</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4760406</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.03574893319570477</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.07149786639140954</v>
+      </c>
+      <c r="G22" t="n">
+        <v>531145</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.1115755672940501</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.8884244327059498</v>
+      </c>
+      <c r="J22" t="n">
+        <v>4229261</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-1138.947116</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1387.48115722136</v>
+      </c>
+      <c r="M22" t="n">
+        <v>4124031</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-7448.881658</v>
+      </c>
+      <c r="O22" t="n">
+        <v>997.079641263684</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-0.082942</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.08534899999999999</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.0002693016855663436</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.004356</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.01811262114178532</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.01811061901835494</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0.01271212232113365</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.0108570798</v>
+      </c>
+      <c r="X22" t="n">
+        <v>-0.054324</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.054337</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>-0.00180621378888762</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>-0.004705</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0.01554905371276285</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0.01544379043859428</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.01148665240440724</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.0103796826</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.05433786342535595</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>4124031</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>1379391</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>2744487</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>104510</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>720</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>105230</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.05996326657797205</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0.01069531241042317</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>-0.020227</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>-0.010551</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>0.004537</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>0.042812</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0.015088</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>-0.020367</v>
+      </c>
+      <c r="AV22" t="n">
+        <v>-0.010755</v>
+      </c>
+      <c r="AW22" t="n">
+        <v>0.00359</v>
+      </c>
+      <c r="AX22" t="n">
+        <v>0.031739</v>
+      </c>
+      <c r="AY22" t="n">
+        <v>0.014345</v>
+      </c>
+      <c r="AZ22" t="n">
+        <v>-0.0002693016855663436</v>
+      </c>
+      <c r="BA22" t="n">
+        <v>0.01811061901835494</v>
+      </c>
+      <c r="BB22" t="n">
+        <v>4403729.871013356</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>4.277117464674753</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0.0900778911541026</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>-0.08294443915333342</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>0.001695789463142083</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>-0.1399415216785829</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>3958657.635908886</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>1.487677549044224</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>2.861796223433792</v>
+      </c>
+      <c r="BK22" t="inlineStr">
+        <is>
+          <t>data\0910-0913\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL22" t="inlineStr">
+        <is>
+          <t>data\0910-0913\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:45:35</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>data\0910-0913</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4760406</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.03574893319570477</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.07149786639140954</v>
+      </c>
+      <c r="G23" t="n">
+        <v>535681</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.112528427197176</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.887471572802824</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4224725</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-5409.197719999998</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1746.962077084208</v>
+      </c>
+      <c r="M23" t="n">
+        <v>4147864</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-10239.362952</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1413.933718417036</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-0.07764699999999999</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.086261</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-0.001280366821509092</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-0.00562</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.02033492225737277</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.02029457375792291</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0.01472730424252466</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0.012935685</v>
+      </c>
+      <c r="X23" t="n">
+        <v>-0.060991</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.061004</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>-0.00246858695270626</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>-0.005869</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0.01846300007708873</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0.01829722520776051</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0.01378183515370803</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0.012520557</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0.06100476677211832</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>4147864</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>1290233</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>2857451</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>75131</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>1730</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>76861</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>0.06284286220580008</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>0.01958672904650037</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>-0.024258</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>-0.013726</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>0.004239</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>0.048816</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0.017965</v>
+      </c>
+      <c r="AU23" t="n">
+        <v>-0.024314</v>
+      </c>
+      <c r="AV23" t="n">
+        <v>-0.013878</v>
+      </c>
+      <c r="AW23" t="n">
+        <v>0.003355</v>
+      </c>
+      <c r="AX23" t="n">
+        <v>0.039944</v>
+      </c>
+      <c r="AY23" t="n">
+        <v>0.017233</v>
+      </c>
+      <c r="AZ23" t="n">
+        <v>-0.001280366821509092</v>
+      </c>
+      <c r="BA23" t="n">
+        <v>0.02029457375792291</v>
+      </c>
+      <c r="BB23" t="n">
+        <v>3504386.087831286</v>
+      </c>
+      <c r="BC23" t="n">
+        <v>3.652603564402182</v>
+      </c>
+      <c r="BD23" t="n">
+        <v>0.08415469159439869</v>
+      </c>
+      <c r="BE23" t="n">
+        <v>-0.07764869258818632</v>
+      </c>
+      <c r="BF23" t="n">
+        <v>-0.0005508193141818829</v>
+      </c>
+      <c r="BG23" t="n">
+        <v>-0.01189603938781511</v>
+      </c>
+      <c r="BH23" t="n">
+        <v>2953163.88135819</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>1.444850968759602</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>2.353973480590835</v>
+      </c>
+      <c r="BK23" t="inlineStr">
+        <is>
+          <t>data\0910-0913\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL23" t="inlineStr">
+        <is>
+          <t>data\0910-0913\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:45:42</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>data\1130-1133</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>107169</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2989573470767932</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2989573470767932</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6481</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.06047457753641445</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.9395254224635855</v>
+      </c>
+      <c r="J24" t="n">
+        <v>100688</v>
+      </c>
+      <c r="K24" t="n">
+        <v>387.4635409999999</v>
+      </c>
+      <c r="L24" t="n">
+        <v>254.320707150435</v>
+      </c>
+      <c r="M24" t="n">
+        <v>99541</v>
+      </c>
+      <c r="N24" t="n">
+        <v>82.56292999999999</v>
+      </c>
+      <c r="O24" t="n">
+        <v>169.413388454264</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-0.142371</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.324587</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.003848160068727156</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.001759</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.0502576299229273</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.05011008909945552</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.03431652611036072</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.0359545326</v>
+      </c>
+      <c r="X24" t="n">
+        <v>-0.142371</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.150625</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.0008294364131362956</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>-0.002246</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.04125464599093457</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.04124630712044288</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.03164888608713997</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0.0354178314</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0.1507728897687819</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>99541</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>47395</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>52146</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>1147</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>1147</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>0.2658244210985178</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>0.05799084710053988</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>-0.063787</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>-0.02464775</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>0.024497</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>0.08058700000000001</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>0.04914475</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>-0.064015</v>
+      </c>
+      <c r="AV24" t="n">
+        <v>-0.024904</v>
+      </c>
+      <c r="AW24" t="n">
+        <v>0.02341</v>
+      </c>
+      <c r="AX24" t="n">
+        <v>0.073939</v>
+      </c>
+      <c r="AY24" t="n">
+        <v>0.048314</v>
+      </c>
+      <c r="AZ24" t="n">
+        <v>0.003848160068727156</v>
+      </c>
+      <c r="BA24" t="n">
+        <v>0.05011008909945552</v>
+      </c>
+      <c r="BB24" t="n">
+        <v>2923929221.325207</v>
+      </c>
+      <c r="BC24" t="n">
+        <v>2.832060979347581</v>
+      </c>
+      <c r="BD24" t="n">
+        <v>0.1629165920718858</v>
+      </c>
+      <c r="BE24" t="n">
+        <v>-0.1424477838120654</v>
+      </c>
+      <c r="BF24" t="n">
+        <v>-0.002755626281185669</v>
+      </c>
+      <c r="BG24" t="n">
+        <v>0.2256086824312147</v>
+      </c>
+      <c r="BH24" t="n">
+        <v>123670007.1303025</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>1.92818300776416</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>9.261362961407954</v>
+      </c>
+      <c r="BK24" t="inlineStr">
+        <is>
+          <t>data\1130-1133\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL24" t="inlineStr">
+        <is>
+          <t>data\1130-1133\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:45:47</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>data\1130-1133</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>107169</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.2989573470767932</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.2989573470767932</v>
+      </c>
+      <c r="G25" t="n">
+        <v>173</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.001614272784107345</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.9983857272158927</v>
+      </c>
+      <c r="J25" t="n">
+        <v>106996</v>
+      </c>
+      <c r="K25" t="n">
+        <v>351.668413</v>
+      </c>
+      <c r="L25" t="n">
+        <v>273.708366389041</v>
+      </c>
+      <c r="M25" t="n">
+        <v>105782</v>
+      </c>
+      <c r="N25" t="n">
+        <v>144.183099</v>
+      </c>
+      <c r="O25" t="n">
+        <v>237.807764522491</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.132015</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.242353</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.003286743551160791</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-0.001021</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.05057783849034463</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.05047093285431021</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.03707921984934016</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.0391584312</v>
+      </c>
+      <c r="X25" t="n">
+        <v>-0.132015</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.151663</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.001363021109451514</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>-0.0015995</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0.04741405817893581</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0.04739446261379803</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0.03554331448639655</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>0.0387307011</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0.1517335154710339</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>105782</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>50991</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>54791</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>1214</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>1214</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>0.1709104728171334</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>0.01902025167563381</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>-0.07968725</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>-0.026851</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0.025967</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>0.09717200000000001</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0.052818</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>-0.0800695</v>
+      </c>
+      <c r="AV25" t="n">
+        <v>-0.027226</v>
+      </c>
+      <c r="AW25" t="n">
+        <v>0.02503675</v>
+      </c>
+      <c r="AX25" t="n">
+        <v>0.089809</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>0.05226275</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>0.003286743551160791</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>0.05047093285431021</v>
+      </c>
+      <c r="BB25" t="n">
+        <v>32964.27991067781</v>
+      </c>
+      <c r="BC25" t="n">
+        <v>2.832868186439337</v>
+      </c>
+      <c r="BD25" t="n">
+        <v>0.1530122898190715</v>
+      </c>
+      <c r="BE25" t="n">
+        <v>-0.1334809517417522</v>
+      </c>
+      <c r="BF25" t="n">
+        <v>-0.00226824427147243</v>
+      </c>
+      <c r="BG25" t="n">
+        <v>0.2253183562047627</v>
+      </c>
+      <c r="BH25" t="n">
+        <v>24618.1070801436</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>0.6353109127584124</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>1.334540595635983</v>
+      </c>
+      <c r="BK25" t="inlineStr">
+        <is>
+          <t>data\1130-1133\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL25" t="inlineStr">
+        <is>
+          <t>data\1130-1133\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:46:14</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>data\1203-1206</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>525255</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.02227102413431687</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.04454204826863374</v>
+      </c>
+      <c r="G26" t="n">
+        <v>83160</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.1583231002084702</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.8416768997915298</v>
+      </c>
+      <c r="J26" t="n">
+        <v>442095</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-1456.103293</v>
+      </c>
+      <c r="L26" t="n">
+        <v>26.426364000355</v>
+      </c>
+      <c r="M26" t="n">
+        <v>440541</v>
+      </c>
+      <c r="N26" t="n">
+        <v>-1451.513524</v>
+      </c>
+      <c r="O26" t="n">
+        <v>25.141339310206</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-0.050102</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.043809</v>
+      </c>
+      <c r="R26" t="n">
+        <v>-0.003293643431841573</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-0.002873</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.007731449166441479</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.006994799436521073</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.005832506531401622</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.006014908199999999</v>
+      </c>
+      <c r="X26" t="n">
+        <v>-0.023187</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.023186</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>-0.003294843213231004</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>-0.00287</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0.007554418462108683</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0.006798032546323539</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0.005753157272535361</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>0.005988221399999999</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0.02319434749932444</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>440541</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>138449</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>301984</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>702</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>852</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>1554</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>-0.002953519305019306</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>0.02860403710562506</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>-0.01621</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>-0.007159</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>0.001015</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>0.007029299999999988</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0.008174000000000001</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>-0.016067</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>-0.007136</v>
+      </c>
+      <c r="AW26" t="n">
+        <v>0.001002</v>
+      </c>
+      <c r="AX26" t="n">
+        <v>0.00693</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>0.008137999999999999</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>-0.003293643431841573</v>
+      </c>
+      <c r="BA26" t="n">
+        <v>0.006994799436521073</v>
+      </c>
+      <c r="BB26" t="n">
+        <v>42346256.51270936</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>6.964052547748475</v>
+      </c>
+      <c r="BD26" t="n">
+        <v>0.04982045808416385</v>
+      </c>
+      <c r="BE26" t="n">
+        <v>-0.05016772148430576</v>
+      </c>
+      <c r="BF26" t="n">
+        <v>-0.001443955549093656</v>
+      </c>
+      <c r="BG26" t="n">
+        <v>-0.4603366504968461</v>
+      </c>
+      <c r="BH26" t="n">
+        <v>12522282637492.26</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>-0.1029800365371982</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>1.301626398854174</v>
+      </c>
+      <c r="BK26" t="inlineStr">
+        <is>
+          <t>data\1203-1206\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL26" t="inlineStr">
+        <is>
+          <t>data\1203-1206\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:46:42</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>data\1203-1206</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>525255</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.02227102413431687</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.04454204826863374</v>
+      </c>
+      <c r="G27" t="n">
+        <v>71420</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.1359720516701412</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8640279483298589</v>
+      </c>
+      <c r="J27" t="n">
+        <v>453835</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-1505.403425</v>
+      </c>
+      <c r="L27" t="n">
+        <v>32.928042210065</v>
+      </c>
+      <c r="M27" t="n">
+        <v>451449</v>
+      </c>
+      <c r="N27" t="n">
+        <v>-1469.98459</v>
+      </c>
+      <c r="O27" t="n">
+        <v>30.967801038202</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-0.033948</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.048227</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-0.003317072118721562</v>
+      </c>
+      <c r="S27" t="n">
+        <v>-0.003121</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.008517927945101322</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.007845516492694287</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.006590852386880694</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.0072691878</v>
+      </c>
+      <c r="X27" t="n">
+        <v>-0.025553</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.025551</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>-0.003256147626863721</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>-0.003094</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0.00828229769177438</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0.007615376398264304</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0.00647548534164435</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0.0072187794</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0.02555378383530396</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>451449</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>149138</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>302185</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>505</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>1881</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>2386</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>-0.01484444048616932</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>0.02451942439195939</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>-0.01685</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>-0.008007</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0.001794</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>0.008583</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0.009801000000000001</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>-0.0163852</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>-0.007936</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>0.001798</v>
+      </c>
+      <c r="AX27" t="n">
+        <v>0.008512</v>
+      </c>
+      <c r="AY27" t="n">
+        <v>0.009734</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>-0.003317072118721562</v>
+      </c>
+      <c r="BA27" t="n">
+        <v>0.007845516492694287</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>27412219.0937402</v>
+      </c>
+      <c r="BC27" t="n">
+        <v>4.241983629205412</v>
+      </c>
+      <c r="BD27" t="n">
+        <v>0.03364629420504441</v>
+      </c>
+      <c r="BE27" t="n">
+        <v>-0.03402716895577954</v>
+      </c>
+      <c r="BF27" t="n">
+        <v>-0.002447119147039802</v>
+      </c>
+      <c r="BG27" t="n">
+        <v>-0.1335771831542694</v>
+      </c>
+      <c r="BH27" t="n">
+        <v>1676855811376.349</v>
+      </c>
+      <c r="BI27" t="n">
+        <v>-0.03192569146630256</v>
+      </c>
+      <c r="BJ27" t="n">
+        <v>0.9610017435193385</v>
+      </c>
+      <c r="BK27" t="inlineStr">
+        <is>
+          <t>data\1203-1206\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL27" t="inlineStr">
+        <is>
+          <t>data\1203-1206\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:50:55</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>data\1306-1311</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>456945</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.3429722222331131</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.6859444444662263</v>
+      </c>
+      <c r="G28" t="n">
+        <v>46325</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.1013798159515916</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8986201840484085</v>
+      </c>
+      <c r="J28" t="n">
+        <v>410620</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-5631.150204</v>
+      </c>
+      <c r="L28" t="n">
+        <v>5283.166335395834</v>
+      </c>
+      <c r="M28" t="n">
+        <v>408013</v>
+      </c>
+      <c r="N28" t="n">
+        <v>-5607.478218000001</v>
+      </c>
+      <c r="O28" t="n">
+        <v>4908.079198452626</v>
+      </c>
+      <c r="P28" t="n">
+        <v>-0.891141</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.54704</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-0.01371377478934294</v>
+      </c>
+      <c r="S28" t="n">
+        <v>-0.010096</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.1134297807928205</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.1125977244518489</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.08589987424869711</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.0969145968</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-0.339924</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.340278</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>-0.01374338125991084</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>-0.010057</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.1096778126810847</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.1088133358832999</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.08403920118231528</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.096183675</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.3402893423784614</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>408013</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>184093</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>223852</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>1258</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>1349</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>2607</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>-0.00908016340621404</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>0.3792024170901793</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>-0.1924053</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>-0.08267099999999999</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>0.049258</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>0.178629</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0.131929</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>-0.189399</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>-0.082109</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>0.048881</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>0.175201</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>0.13099</v>
+      </c>
+      <c r="AZ28" t="n">
+        <v>-0.01371377478934294</v>
+      </c>
+      <c r="BA28" t="n">
+        <v>0.1125977244518489</v>
+      </c>
+      <c r="BB28" t="n">
+        <v>55344718622.40401</v>
+      </c>
+      <c r="BC28" t="n">
+        <v>5.469406961672933</v>
+      </c>
+      <c r="BD28" t="n">
+        <v>0.6298677156506114</v>
+      </c>
+      <c r="BE28" t="n">
+        <v>-0.597542929178331</v>
+      </c>
+      <c r="BF28" t="n">
+        <v>0.009495898092362176</v>
+      </c>
+      <c r="BG28" t="n">
+        <v>-0.3145640869273533</v>
+      </c>
+      <c r="BH28" t="n">
+        <v>31354953.9692882</v>
+      </c>
+      <c r="BI28" t="n">
+        <v>0.1257277743017294</v>
+      </c>
+      <c r="BJ28" t="n">
+        <v>0.8053279620447</v>
+      </c>
+      <c r="BK28" t="inlineStr">
+        <is>
+          <t>data\1306-1311\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL28" t="inlineStr">
+        <is>
+          <t>data\1306-1311\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-26 15:55:15</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>data\1306-1311</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>456945</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.3429722222331131</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.6859444444662263</v>
+      </c>
+      <c r="G29" t="n">
+        <v>46247</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.1012091170709823</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.8987908829290177</v>
+      </c>
+      <c r="J29" t="n">
+        <v>410698</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-10609.961491</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5864.885256735723</v>
+      </c>
+      <c r="M29" t="n">
+        <v>408878</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-10601.824566</v>
+      </c>
+      <c r="O29" t="n">
+        <v>5587.144379409167</v>
+      </c>
+      <c r="P29" t="n">
+        <v>-0.593645</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.552206</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-0.0258339740904509</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-0.026103</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.11950015426565</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.1166743015929732</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.09163510781401417</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.099571416</v>
+      </c>
+      <c r="X29" t="n">
+        <v>-0.358434</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.358315</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-0.02592906579957836</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>-0.026096</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0.1168955760114977</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.1139835919675327</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.09030980355998611</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.09892426110000001</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0.35850046279695</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>408878</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>158071</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>250747</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>896</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>924</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>1820</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>-0.004470837912087923</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>0.3906211582343156</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>-0.19952705</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>-0.103399</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>0.033741</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0.18593</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0.13714</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>-0.19752635</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>-0.10287</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>0.03337125</v>
+      </c>
+      <c r="AX29" t="n">
+        <v>0.182314</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>0.13624125</v>
+      </c>
+      <c r="AZ29" t="n">
+        <v>-0.0258339740904509</v>
+      </c>
+      <c r="BA29" t="n">
+        <v>0.1166743015929732</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>47495.86749110976</v>
+      </c>
+      <c r="BC29" t="n">
+        <v>5.024446422859851</v>
+      </c>
+      <c r="BD29" t="n">
+        <v>0.615434017231729</v>
+      </c>
+      <c r="BE29" t="n">
+        <v>-0.5937890083506836</v>
+      </c>
+      <c r="BF29" t="n">
+        <v>-0.004946881075369225</v>
+      </c>
+      <c r="BG29" t="n">
+        <v>-0.2574889898994292</v>
+      </c>
+      <c r="BH29" t="n">
+        <v>1765701.973573729</v>
+      </c>
+      <c r="BI29" t="n">
+        <v>0.382199500314065</v>
+      </c>
+      <c r="BJ29" t="n">
+        <v>0.8067670926329948</v>
+      </c>
+      <c r="BK29" t="inlineStr">
+        <is>
+          <t>data\1306-1311\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL29" t="inlineStr">
+        <is>
+          <t>data\1306-1311\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:03:56</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.06227940749394916</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="G30" t="n">
+        <v>9634</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.01358569961981476</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.9864143003801853</v>
+      </c>
+      <c r="J30" t="n">
+        <v>699494</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-621.7036519999999</v>
+      </c>
+      <c r="L30" t="n">
+        <v>143.812791320498</v>
+      </c>
+      <c r="M30" t="n">
+        <v>683858</v>
+      </c>
+      <c r="N30" t="n">
+        <v>-1245.446727</v>
+      </c>
+      <c r="O30" t="n">
+        <v>89.512016083193</v>
+      </c>
+      <c r="P30" t="n">
+        <v>-0.11556</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.132246</v>
+      </c>
+      <c r="R30" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="S30" t="n">
+        <v>-0.002101</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.01433860038117433</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.009318774988777602</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.008409307199999999</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-0.043002</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.043009</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>-0.001821206635003173</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>-0.002249</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0.01144083450710502</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.0112949502261668</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.008215368975723031</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.008176539</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0.04301580114352299</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>683858</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>264076</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>419712</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>12902</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>2734</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>15636</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>0.03989147320286518</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>0.04337597406792291</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>-0.018882</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>-0.007848000000000001</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>0.003504</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>0.024597</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0.011352</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>-0.018424</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>-0.007889</v>
+      </c>
+      <c r="AW30" t="n">
+        <v>0.003141</v>
+      </c>
+      <c r="AX30" t="n">
+        <v>0.018931</v>
+      </c>
+      <c r="AY30" t="n">
+        <v>0.01103</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>238689480875.462</v>
+      </c>
+      <c r="BC30" t="n">
+        <v>5.675151041459209</v>
+      </c>
+      <c r="BD30" t="n">
+        <v>0.1035729672089861</v>
+      </c>
+      <c r="BE30" t="n">
+        <v>-0.09813477944421571</v>
+      </c>
+      <c r="BF30" t="n">
+        <v>0.001960367063261137</v>
+      </c>
+      <c r="BG30" t="n">
+        <v>-0.338411737141495</v>
+      </c>
+      <c r="BH30" t="n">
+        <v>9860681782068.098</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>1.553251175032938</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>7.219025590519583</v>
+      </c>
+      <c r="BK30" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL30" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:06:07</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.06227940749394916</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="G31" t="n">
+        <v>9634</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.01358569961981476</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.9864143003801853</v>
+      </c>
+      <c r="J31" t="n">
+        <v>699494</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-621.7036519999999</v>
+      </c>
+      <c r="L31" t="n">
+        <v>143.812791320498</v>
+      </c>
+      <c r="M31" t="n">
+        <v>683858</v>
+      </c>
+      <c r="N31" t="n">
+        <v>-1245.446727</v>
+      </c>
+      <c r="O31" t="n">
+        <v>89.512016083193</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-0.11556</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.132246</v>
+      </c>
+      <c r="R31" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="S31" t="n">
+        <v>-0.002101</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.01433860038117433</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.009318774988777602</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.008409307199999999</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-0.043002</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.043009</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>-0.001821206635003173</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>-0.002249</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.01144083450710502</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.0112949502261668</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.008215368975723031</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.008176539</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0.04301580114352299</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>683858</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>264076</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>419712</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>12902</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>2734</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>15636</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>0.03989147320286518</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>0.04337597406792291</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>-0.018882</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>-0.007848000000000001</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>0.003504</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>0.024597</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0.011352</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>-0.018424</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>-0.007889</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>0.003141</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>0.018931</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>0.01103</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="BB31" t="n">
+        <v>238689480875.462</v>
+      </c>
+      <c r="BC31" t="n">
+        <v>5.675151041459209</v>
+      </c>
+      <c r="BD31" t="n">
+        <v>0.1035729672089861</v>
+      </c>
+      <c r="BE31" t="n">
+        <v>-0.09813477944421571</v>
+      </c>
+      <c r="BF31" t="n">
+        <v>0.001960367063261137</v>
+      </c>
+      <c r="BG31" t="n">
+        <v>-0.338411737141495</v>
+      </c>
+      <c r="BH31" t="n">
+        <v>9860681782068.098</v>
+      </c>
+      <c r="BI31" t="n">
+        <v>1.553251175032938</v>
+      </c>
+      <c r="BJ31" t="n">
+        <v>7.219025590519583</v>
+      </c>
+      <c r="BK31" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL31" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:06:37</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.06227940749394916</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="G32" t="n">
+        <v>22506</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.03173757065015061</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.9682624293498494</v>
+      </c>
+      <c r="J32" t="n">
+        <v>686622</v>
+      </c>
+      <c r="K32" t="n">
+        <v>69903.96206200001</v>
+      </c>
+      <c r="L32" t="n">
+        <v>7732.276593232876</v>
+      </c>
+      <c r="M32" t="n">
+        <v>686622</v>
+      </c>
+      <c r="N32" t="n">
+        <v>69903.96206200001</v>
+      </c>
+      <c r="O32" t="n">
+        <v>7732.276593232876</v>
+      </c>
+      <c r="P32" t="n">
+        <v>-0.177462</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.16966</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.110818</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.106119411577341</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.1036619853806024</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.0108407712</v>
+      </c>
+      <c r="X32" t="n">
+        <v>-0.177462</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.16966</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0.110818</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.106119411577341</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.1036619853806024</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.0108407712</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0.3183582347320229</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>686622</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>672373</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>14179</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0.042818</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>0.100664</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>0.116521</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>0.122748</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0.015857</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>0.042818</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>0.100664</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>0.116521</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>0.122748</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>0.015857</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>376683105753783</v>
+      </c>
+      <c r="BC32" t="n">
+        <v>3116461253.414898</v>
+      </c>
+      <c r="BD32" t="n">
+        <v>44696799.24024205</v>
+      </c>
+      <c r="BE32" t="n">
+        <v>-44696799.12847926</v>
+      </c>
+      <c r="BF32" t="n">
+        <v>0.1117627918720245</v>
+      </c>
+      <c r="BH32" t="n">
+        <v>143288461696.1187</v>
+      </c>
+      <c r="BI32" t="n">
+        <v>-3.511182407813983</v>
+      </c>
+      <c r="BJ32" t="n">
+        <v>15.83006628916045</v>
+      </c>
+      <c r="BK32" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL32" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:07:11</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>data\0817-0821</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>4524729</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0582136383980279</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.0582136383980279</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4059637</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.8972110815918478</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.1027889184081522</v>
+      </c>
+      <c r="J33" t="n">
+        <v>465092</v>
+      </c>
+      <c r="K33" t="n">
+        <v>976.6259189999996</v>
+      </c>
+      <c r="L33" t="n">
+        <v>463.755326179349</v>
+      </c>
+      <c r="M33" t="n">
+        <v>465092</v>
+      </c>
+      <c r="N33" t="n">
+        <v>976.6259189999996</v>
+      </c>
+      <c r="O33" t="n">
+        <v>463.755326179349</v>
+      </c>
+      <c r="P33" t="n">
+        <v>-0.08731899999999999</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.075143</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.002099855338298658</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.000682</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.03157730199467438</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.03150740561869677</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.0268029508505844</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.037843365</v>
+      </c>
+      <c r="X33" t="n">
+        <v>-0.08731899999999999</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.075143</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.002099855338298658</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.000682</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.03157730199467438</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.03150740561869677</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.0268029508505844</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.037843365</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0.09473190598402315</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>465092</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>236205</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>228887</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>-0.049175</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>-0.021687</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>0.02967</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>0.052074</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0.051357</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>-0.049175</v>
+      </c>
+      <c r="AV33" t="n">
+        <v>-0.021687</v>
+      </c>
+      <c r="AW33" t="n">
+        <v>0.02967</v>
+      </c>
+      <c r="AX33" t="n">
+        <v>0.052074</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>0.051357</v>
+      </c>
+      <c r="AZ33" t="n">
+        <v>0.002099855338298658</v>
+      </c>
+      <c r="BA33" t="n">
+        <v>0.03150740561869677</v>
+      </c>
+      <c r="BB33" t="n">
+        <v>130149.1526970406</v>
+      </c>
+      <c r="BC33" t="n">
+        <v>3.186243312399336</v>
+      </c>
+      <c r="BD33" t="n">
+        <v>0.100257482019355</v>
+      </c>
+      <c r="BE33" t="n">
+        <v>-0.08743992219000901</v>
+      </c>
+      <c r="BF33" t="n">
+        <v>0.00163946024401361</v>
+      </c>
+      <c r="BG33" t="n">
+        <v>0.1104176033939543</v>
+      </c>
+      <c r="BH33" t="n">
+        <v>117765.9006510912</v>
+      </c>
+      <c r="BI33" t="n">
+        <v>0.007020067219647775</v>
+      </c>
+      <c r="BJ33" t="n">
+        <v>-1.029210864122549</v>
+      </c>
+      <c r="BK33" t="inlineStr">
+        <is>
+          <t>data\0817-0821\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL33" t="inlineStr">
+        <is>
+          <t>data\0817-0821\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:07:33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>data\0817-0821</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>4524729</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0582136383980279</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.0582136383980279</v>
+      </c>
+      <c r="G34" t="n">
+        <v>4033600</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.8914567038158528</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.1085432961841472</v>
+      </c>
+      <c r="J34" t="n">
+        <v>491129</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3464.355936</v>
+      </c>
+      <c r="L34" t="n">
+        <v>527.7055922894559</v>
+      </c>
+      <c r="M34" t="n">
+        <v>491129</v>
+      </c>
+      <c r="N34" t="n">
+        <v>3464.355936</v>
+      </c>
+      <c r="O34" t="n">
+        <v>527.7055922894559</v>
+      </c>
+      <c r="P34" t="n">
+        <v>-0.08332299999999999</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.08219600000000001</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.007053861482421116</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.011646</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.03277917801531105</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.03201120974824705</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.02848910105084408</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.03868992959999999</v>
+      </c>
+      <c r="X34" t="n">
+        <v>-0.08332299999999999</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.08219600000000001</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0.007053861482421116</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0.011646</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0.03277917801531105</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.03201120974824705</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0.02848910105084408</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0.03868992959999999</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0.09833753404593315</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>491129</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>301525</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>189590</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>-0.048314</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>-0.018747</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>0.034025</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>0.052714</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>0.052772</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>-0.048314</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>-0.018747</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>0.034025</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>0.052714</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>0.052772</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>0.007053861482421116</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>0.03201120974824705</v>
+      </c>
+      <c r="BB34" t="n">
+        <v>162003.3002031418</v>
+      </c>
+      <c r="BC34" t="n">
+        <v>6.558509808319927</v>
+      </c>
+      <c r="BD34" t="n">
+        <v>0.1882205188032683</v>
+      </c>
+      <c r="BE34" t="n">
+        <v>-0.1679930739191043</v>
+      </c>
+      <c r="BF34" t="n">
+        <v>0.0155391056352138</v>
+      </c>
+      <c r="BG34" t="n">
+        <v>-0.426334682974276</v>
+      </c>
+      <c r="BH34" t="n">
+        <v>143418.1181615088</v>
+      </c>
+      <c r="BI34" t="n">
+        <v>-0.3084677670383042</v>
+      </c>
+      <c r="BJ34" t="n">
+        <v>-1.002580762690497</v>
+      </c>
+      <c r="BK34" t="inlineStr">
+        <is>
+          <t>data\0817-0821\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL34" t="inlineStr">
+        <is>
+          <t>data\0817-0821\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:10:55</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.06227940749394916</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="G35" t="n">
+        <v>9634</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.01358569961981476</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.9864143003801853</v>
+      </c>
+      <c r="J35" t="n">
+        <v>699494</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-621.7036519999999</v>
+      </c>
+      <c r="L35" t="n">
+        <v>143.812791320498</v>
+      </c>
+      <c r="M35" t="n">
+        <v>697268</v>
+      </c>
+      <c r="N35" t="n">
+        <v>-783.3721039999998</v>
+      </c>
+      <c r="O35" t="n">
+        <v>129.213430730248</v>
+      </c>
+      <c r="P35" t="n">
+        <v>-0.11556</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.132246</v>
+      </c>
+      <c r="R35" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="S35" t="n">
+        <v>-0.002101</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.01433860038117433</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.009318774988777602</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.008409307199999999</v>
+      </c>
+      <c r="X35" t="n">
+        <v>-0.070997</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0.071673</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>-0.001123487818170344</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>-0.002132</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0.01361300366876381</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0.01356656345609307</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0.009091752694803145</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0.008378172599999999</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0.07169300190587165</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>697268</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>274857</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>422341</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>2121</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>105</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>2226</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>0.07262733692722372</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>0.0358306103753022</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>-0.018882</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>-0.007848000000000001</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>0.003504</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>0.024597</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>0.011352</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>-0.018883</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>-0.007863999999999999</v>
+      </c>
+      <c r="AW35" t="n">
+        <v>0.003446</v>
+      </c>
+      <c r="AX35" t="n">
+        <v>0.023499</v>
+      </c>
+      <c r="AY35" t="n">
+        <v>0.01131</v>
+      </c>
+      <c r="AZ35" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="BA35" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="BB35" t="n">
+        <v>238689480875.462</v>
+      </c>
+      <c r="BC35" t="n">
+        <v>5.675151041459209</v>
+      </c>
+      <c r="BD35" t="n">
+        <v>0.1035729672089861</v>
+      </c>
+      <c r="BE35" t="n">
+        <v>-0.09813477944421571</v>
+      </c>
+      <c r="BF35" t="n">
+        <v>0.001960367063261137</v>
+      </c>
+      <c r="BG35" t="n">
+        <v>-0.338411737141495</v>
+      </c>
+      <c r="BH35" t="n">
+        <v>9860681782068.098</v>
+      </c>
+      <c r="BI35" t="n">
+        <v>1.553251175032938</v>
+      </c>
+      <c r="BJ35" t="n">
+        <v>7.219025590519583</v>
+      </c>
+      <c r="BK35" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL35" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-08-26 16:11:24</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>data\0342-0349</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ref_ai</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.06227940749394916</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="G36" t="n">
+        <v>22506</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.03173757065015061</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.9682624293498494</v>
+      </c>
+      <c r="J36" t="n">
+        <v>686622</v>
+      </c>
+      <c r="K36" t="n">
+        <v>69903.96206200001</v>
+      </c>
+      <c r="L36" t="n">
+        <v>7732.276593232876</v>
+      </c>
+      <c r="M36" t="n">
+        <v>686622</v>
+      </c>
+      <c r="N36" t="n">
+        <v>69903.96206200001</v>
+      </c>
+      <c r="O36" t="n">
+        <v>7732.276593232876</v>
+      </c>
+      <c r="P36" t="n">
+        <v>-0.177462</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.16966</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.110818</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.106119411577341</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0.1036619853806024</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0.0108407712</v>
+      </c>
+      <c r="X36" t="n">
+        <v>-0.177462</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0.16966</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>0.110818</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>0.106119411577341</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>0.1036619853806024</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>0.0108407712</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>0.5305970578867049</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>686622</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>672373</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>14179</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN36" t="n">
+        <v/>
+      </c>
+      <c r="AO36" t="n">
+        <v/>
+      </c>
+      <c r="AP36" t="n">
+        <v>0.042818</v>
+      </c>
+      <c r="AQ36" t="n">
+        <v>0.100664</v>
+      </c>
+      <c r="AR36" t="n">
+        <v>0.116521</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>0.122748</v>
+      </c>
+      <c r="AT36" t="n">
+        <v>0.015857</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>0.042818</v>
+      </c>
+      <c r="AV36" t="n">
+        <v>0.100664</v>
+      </c>
+      <c r="AW36" t="n">
+        <v>0.116521</v>
+      </c>
+      <c r="AX36" t="n">
+        <v>0.122748</v>
+      </c>
+      <c r="AY36" t="n">
+        <v>0.015857</v>
+      </c>
+      <c r="AZ36" t="n">
+        <v>0.1018085089933035</v>
+      </c>
+      <c r="BA36" t="n">
+        <v>0.0299392219351395</v>
+      </c>
+      <c r="BB36" t="n">
+        <v>376683105753783</v>
+      </c>
+      <c r="BC36" t="n">
+        <v>3116461253.414898</v>
+      </c>
+      <c r="BD36" t="n">
+        <v>44696799.24024205</v>
+      </c>
+      <c r="BE36" t="n">
+        <v>-44696799.12847926</v>
+      </c>
+      <c r="BF36" t="n">
+        <v>0.1117627918720245</v>
+      </c>
+      <c r="BG36" t="n">
+        <v/>
+      </c>
+      <c r="BH36" t="n">
+        <v>143288461696.1187</v>
+      </c>
+      <c r="BI36" t="n">
+        <v>-3.511182407813983</v>
+      </c>
+      <c r="BJ36" t="n">
+        <v>15.83006628916045</v>
+      </c>
+      <c r="BK36" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_ai_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BL36" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BD20">
     <sortState ref="A2:BC25">

</xml_diff>

<commit_message>
chore: Add VSCode settings for pytest and update configuration parameters in JSON files
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -737,7 +737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM69"/>
+  <dimension ref="A1:BM71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
@@ -15005,9 +15005,6 @@
       <c r="BG69" t="n">
         <v>0.1117627918720245</v>
       </c>
-      <c r="BH69" t="n">
-        <v/>
-      </c>
       <c r="BI69" t="n">
         <v>143288461696.1187</v>
       </c>
@@ -15025,6 +15022,424 @@
       <c r="BM69" t="inlineStr">
         <is>
           <t>data\0342-0349\python_ref_ai_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-09-01 17:21:35</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>0342-0349</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>mov.ply-ref.ply</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>27711</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.04022176252969904</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.08044352505939807</v>
+      </c>
+      <c r="G70" t="n">
+        <v>116</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.004186063296163978</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.995813936703836</v>
+      </c>
+      <c r="J70" t="n">
+        <v>27595</v>
+      </c>
+      <c r="K70" t="n">
+        <v>-66.313918</v>
+      </c>
+      <c r="L70" t="n">
+        <v>4.678322496426</v>
+      </c>
+      <c r="M70" t="n">
+        <v>27230</v>
+      </c>
+      <c r="N70" t="n">
+        <v>-76.54673100000001</v>
+      </c>
+      <c r="O70" t="n">
+        <v>3.851327580325</v>
+      </c>
+      <c r="P70" t="n">
+        <v>-0.088936</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0.067135</v>
+      </c>
+      <c r="R70" t="n">
+        <v>-0.002403113535060699</v>
+      </c>
+      <c r="S70" t="n">
+        <v>-0.002479</v>
+      </c>
+      <c r="T70" t="n">
+        <v>0.01302056646870666</v>
+      </c>
+      <c r="U70" t="n">
+        <v>0.01279688229623202</v>
+      </c>
+      <c r="V70" t="n">
+        <v>0.009201061061786555</v>
+      </c>
+      <c r="W70" t="n">
+        <v>0.008914873799999999</v>
+      </c>
+      <c r="X70" t="n">
+        <v>-0.038914</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>0.039006</v>
+      </c>
+      <c r="Z70" t="n">
+        <v>-0.002811117554168197</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>-0.002606</v>
+      </c>
+      <c r="AB70" t="n">
+        <v>0.01189272589166281</v>
+      </c>
+      <c r="AC70" t="n">
+        <v>0.01155571491647637</v>
+      </c>
+      <c r="AD70" t="n">
+        <v>0.008694125045905252</v>
+      </c>
+      <c r="AE70" t="n">
+        <v>0.008712498900000001</v>
+      </c>
+      <c r="AF70" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG70" t="n">
+        <v>0.03906169940611999</v>
+      </c>
+      <c r="AH70" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI70" t="n">
+        <v>27230</v>
+      </c>
+      <c r="AJ70" t="n">
+        <v>8999</v>
+      </c>
+      <c r="AK70" t="n">
+        <v>16614</v>
+      </c>
+      <c r="AL70" t="n">
+        <v>286</v>
+      </c>
+      <c r="AM70" t="n">
+        <v>79</v>
+      </c>
+      <c r="AN70" t="n">
+        <v>365</v>
+      </c>
+      <c r="AO70" t="n">
+        <v>0.02803510410958904</v>
+      </c>
+      <c r="AP70" t="n">
+        <v>0.03846781035790349</v>
+      </c>
+      <c r="AQ70" t="n">
+        <v>-0.0208045</v>
+      </c>
+      <c r="AR70" t="n">
+        <v>-0.009398</v>
+      </c>
+      <c r="AS70" t="n">
+        <v>0.002544</v>
+      </c>
+      <c r="AT70" t="n">
+        <v>0.021122</v>
+      </c>
+      <c r="AU70" t="n">
+        <v>0.011942</v>
+      </c>
+      <c r="AV70" t="n">
+        <v>-0.020469</v>
+      </c>
+      <c r="AW70" t="n">
+        <v>-0.009423249999999999</v>
+      </c>
+      <c r="AX70" t="n">
+        <v>0.002283</v>
+      </c>
+      <c r="AY70" t="n">
+        <v>0.018149</v>
+      </c>
+      <c r="AZ70" t="n">
+        <v>0.01170625</v>
+      </c>
+      <c r="BA70" t="n">
+        <v>-0.002403113535060699</v>
+      </c>
+      <c r="BB70" t="n">
+        <v>0.01279688229623202</v>
+      </c>
+      <c r="BC70" t="n">
+        <v>55192845.10587456</v>
+      </c>
+      <c r="BD70" t="n">
+        <v>5.055060238338491</v>
+      </c>
+      <c r="BE70" t="n">
+        <v>0.07339386442785875</v>
+      </c>
+      <c r="BF70" t="n">
+        <v>-0.07048613170858216</v>
+      </c>
+      <c r="BG70" t="n">
+        <v>-0.0002238112750802268</v>
+      </c>
+      <c r="BH70" t="n">
+        <v>-0.2616825721550063</v>
+      </c>
+      <c r="BI70" t="n">
+        <v>101382149.497469</v>
+      </c>
+      <c r="BJ70" t="n">
+        <v>0.7945330257039492</v>
+      </c>
+      <c r="BK70" t="n">
+        <v>3.182318231360224</v>
+      </c>
+      <c r="BL70" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov.ply-ref.ply_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM70" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov.ply-ref.ply_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-09-01 17:31:27</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>0342-0349</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>mov-ref</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G71" t="n">
+        <v>95</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J71" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K71" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L71" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M71" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N71" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O71" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P71" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R71" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S71" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T71" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U71" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V71" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W71" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X71" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z71" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB71" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC71" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD71" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE71" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF71" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG71" t="n">
+        <v>0.04388567971555496</v>
+      </c>
+      <c r="AH71" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI71" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AJ71" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AK71" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AL71" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AM71" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AN71" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AO71" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AP71" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AQ71" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AR71" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AS71" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AT71" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AU71" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AV71" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AW71" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AX71" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AY71" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AZ71" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="BA71" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="BB71" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="BC71" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BD71" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BE71" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BF71" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BG71" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BH71" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BI71" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BJ71" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BK71" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BL71" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM71" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_params.txt</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance M3C2 Processing and Outlier Handling
- Added logging for processing Python distances and parameters in StatisticsService.
- Updated BatchOrchestrator to return distances, uncertainties, and distances path from M3C2 execution.
- Modified OutlierHandler to accept distances path for outlier exclusion, improving clarity and functionality.
- Adjusted M3C2Executor to return the distances path along with distances and uncertainties.
- Updated tests to include logging for savefig calls in outlier plots.
- Updated binary output file for MARS statistics.
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -737,7 +737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM71"/>
+  <dimension ref="A1:BM73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
@@ -15443,6 +15443,424 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-09-02 10:47:55</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0342-0349</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>mov-ref</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1245588149878983</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.2491176299757966</v>
+      </c>
+      <c r="G72" t="n">
+        <v>95</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.00013396735145136</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.9998660326485487</v>
+      </c>
+      <c r="J72" t="n">
+        <v>709033</v>
+      </c>
+      <c r="K72" t="n">
+        <v>-151.9928180000001</v>
+      </c>
+      <c r="L72" t="n">
+        <v>151.729350141048</v>
+      </c>
+      <c r="M72" t="n">
+        <v>690813</v>
+      </c>
+      <c r="N72" t="n">
+        <v>-1125.949142</v>
+      </c>
+      <c r="O72" t="n">
+        <v>62.170601304942</v>
+      </c>
+      <c r="P72" t="n">
+        <v>-0.120008</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0.134913</v>
+      </c>
+      <c r="R72" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="S72" t="n">
+        <v>-0.002299</v>
+      </c>
+      <c r="T72" t="n">
+        <v>0.01462855990518499</v>
+      </c>
+      <c r="U72" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="V72" t="n">
+        <v>0.008219008269008636</v>
+      </c>
+      <c r="W72" t="n">
+        <v>0.006827373</v>
+      </c>
+      <c r="X72" t="n">
+        <v>-0.043862</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>0.043885</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>-0.00162988991521584</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>-0.002469</v>
+      </c>
+      <c r="AB72" t="n">
+        <v>0.009486637003424522</v>
+      </c>
+      <c r="AC72" t="n">
+        <v>0.009345573310344375</v>
+      </c>
+      <c r="AD72" t="n">
+        <v>0.006657630840762984</v>
+      </c>
+      <c r="AE72" t="n">
+        <v>0.0065990526</v>
+      </c>
+      <c r="AF72" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG72" t="n">
+        <v>0.04388567971555496</v>
+      </c>
+      <c r="AH72" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI72" t="n">
+        <v>690813</v>
+      </c>
+      <c r="AJ72" t="n">
+        <v>246292</v>
+      </c>
+      <c r="AK72" t="n">
+        <v>444509</v>
+      </c>
+      <c r="AL72" t="n">
+        <v>15929</v>
+      </c>
+      <c r="AM72" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AN72" t="n">
+        <v>18220</v>
+      </c>
+      <c r="AO72" t="n">
+        <v>0.05345534160263447</v>
+      </c>
+      <c r="AP72" t="n">
+        <v>0.04536447157847037</v>
+      </c>
+      <c r="AQ72" t="n">
+        <v>-0.013568</v>
+      </c>
+      <c r="AR72" t="n">
+        <v>-0.006508</v>
+      </c>
+      <c r="AS72" t="n">
+        <v>0.002725</v>
+      </c>
+      <c r="AT72" t="n">
+        <v>0.022282</v>
+      </c>
+      <c r="AU72" t="n">
+        <v>0.009233</v>
+      </c>
+      <c r="AV72" t="n">
+        <v>-0.013419</v>
+      </c>
+      <c r="AW72" t="n">
+        <v>-0.006579</v>
+      </c>
+      <c r="AX72" t="n">
+        <v>0.002358</v>
+      </c>
+      <c r="AY72" t="n">
+        <v>0.013891</v>
+      </c>
+      <c r="AZ72" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="BA72" t="n">
+        <v>-0.0002143663524828888</v>
+      </c>
+      <c r="BB72" t="n">
+        <v>0.01462698916272617</v>
+      </c>
+      <c r="BC72" t="n">
+        <v>32673381941410.1</v>
+      </c>
+      <c r="BD72" t="n">
+        <v>1.010085389383569</v>
+      </c>
+      <c r="BE72" t="n">
+        <v>0.3498892426805521</v>
+      </c>
+      <c r="BF72" t="n">
+        <v>-0.09252700291488647</v>
+      </c>
+      <c r="BG72" t="n">
+        <v>-0.08886902402080391</v>
+      </c>
+      <c r="BH72" t="n">
+        <v>1.970131977073834</v>
+      </c>
+      <c r="BI72" t="n">
+        <v>11637763.60543192</v>
+      </c>
+      <c r="BJ72" t="n">
+        <v>2.908214737699866</v>
+      </c>
+      <c r="BK72" t="n">
+        <v>16.58429873827257</v>
+      </c>
+      <c r="BL72" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM72" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-09-02 10:59:42</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0342-0349</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>mov-ref</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.0622794074939492</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.124558814987898</v>
+      </c>
+      <c r="G73" t="n">
+        <v>9634</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.01358569961981476</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.9864143003801853</v>
+      </c>
+      <c r="J73" t="n">
+        <v>699494</v>
+      </c>
+      <c r="K73" t="n">
+        <v>-621.7036519999999</v>
+      </c>
+      <c r="L73" t="n">
+        <v>143.812791320498</v>
+      </c>
+      <c r="M73" t="n">
+        <v>683858</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-1245.446727</v>
+      </c>
+      <c r="O73" t="n">
+        <v>89.512016083193</v>
+      </c>
+      <c r="P73" t="n">
+        <v>-0.11556</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.132246</v>
+      </c>
+      <c r="R73" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="S73" t="n">
+        <v>-0.002101</v>
+      </c>
+      <c r="T73" t="n">
+        <v>0.01433860038117433</v>
+      </c>
+      <c r="U73" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="V73" t="n">
+        <v>0.009318774988777602</v>
+      </c>
+      <c r="W73" t="n">
+        <v>0.008409307199999999</v>
+      </c>
+      <c r="X73" t="n">
+        <v>-0.043002</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>0.043009</v>
+      </c>
+      <c r="Z73" t="n">
+        <v>-0.001821206635003173</v>
+      </c>
+      <c r="AA73" t="n">
+        <v>-0.002249</v>
+      </c>
+      <c r="AB73" t="n">
+        <v>0.01144083450710502</v>
+      </c>
+      <c r="AC73" t="n">
+        <v>0.0112949502261668</v>
+      </c>
+      <c r="AD73" t="n">
+        <v>0.008215368975723031</v>
+      </c>
+      <c r="AE73" t="n">
+        <v>0.008176539</v>
+      </c>
+      <c r="AF73" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG73" t="n">
+        <v>0.04301580114352299</v>
+      </c>
+      <c r="AH73" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI73" t="n">
+        <v>683858</v>
+      </c>
+      <c r="AJ73" t="n">
+        <v>264076</v>
+      </c>
+      <c r="AK73" t="n">
+        <v>419712</v>
+      </c>
+      <c r="AL73" t="n">
+        <v>12902</v>
+      </c>
+      <c r="AM73" t="n">
+        <v>2734</v>
+      </c>
+      <c r="AN73" t="n">
+        <v>15636</v>
+      </c>
+      <c r="AO73" t="n">
+        <v>0.03989147320286518</v>
+      </c>
+      <c r="AP73" t="n">
+        <v>0.04337597406792291</v>
+      </c>
+      <c r="AQ73" t="n">
+        <v>-0.018882</v>
+      </c>
+      <c r="AR73" t="n">
+        <v>-0.007848000000000001</v>
+      </c>
+      <c r="AS73" t="n">
+        <v>0.003504</v>
+      </c>
+      <c r="AT73" t="n">
+        <v>0.024597</v>
+      </c>
+      <c r="AU73" t="n">
+        <v>0.011352</v>
+      </c>
+      <c r="AV73" t="n">
+        <v>-0.018424</v>
+      </c>
+      <c r="AW73" t="n">
+        <v>-0.007889</v>
+      </c>
+      <c r="AX73" t="n">
+        <v>0.003141</v>
+      </c>
+      <c r="AY73" t="n">
+        <v>0.018931</v>
+      </c>
+      <c r="AZ73" t="n">
+        <v>0.01103</v>
+      </c>
+      <c r="BA73" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="BB73" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="BC73" t="n">
+        <v>238689480875.462</v>
+      </c>
+      <c r="BD73" t="n">
+        <v>5.675151041459209</v>
+      </c>
+      <c r="BE73" t="n">
+        <v>0.1035729672089861</v>
+      </c>
+      <c r="BF73" t="n">
+        <v>-0.09813477944421571</v>
+      </c>
+      <c r="BG73" t="n">
+        <v>0.001960367063261137</v>
+      </c>
+      <c r="BH73" t="n">
+        <v>-0.338411737141495</v>
+      </c>
+      <c r="BI73" t="n">
+        <v>9860681782068.098</v>
+      </c>
+      <c r="BJ73" t="n">
+        <v>1.553251175032938</v>
+      </c>
+      <c r="BK73" t="n">
+        <v>7.219025590519583</v>
+      </c>
+      <c r="BL73" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM73" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BE21">
     <sortState ref="A2:BC25">

</xml_diff>

<commit_message>
Add support for single cloud statistics processing
- Introduced a new command-line argument `--filename_singlestats` to specify the single statistics file.
- Updated the `DataSourceConfig` and `PipelineConfig` classes to include `filename_singlecloud`.
- Modified the `StatisticsService` to handle single cloud statistics calculations.
- Enhanced the `DataLoader` to load single cloud data based on the provided configuration.
- Updated the `BatchOrchestrator` to manage both multi-cloud and single-cloud data loading.
- Refactored the `StatisticsRunner` to compute statistics for single clouds separately.
- Added logging for better traceability during the loading and processing of point clouds.
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_distances.xlsx
@@ -737,7 +737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM74"/>
+  <dimension ref="A1:BM75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
@@ -16070,6 +16070,215 @@
         </is>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-09-02 13:45:05</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>0342-0349</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>mov-ref</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>709128</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.0622794074939492</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.124558814987898</v>
+      </c>
+      <c r="G75" t="n">
+        <v>9634</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.01358569961981476</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.9864143003801853</v>
+      </c>
+      <c r="J75" t="n">
+        <v>699494</v>
+      </c>
+      <c r="K75" t="n">
+        <v>-621.7036519999999</v>
+      </c>
+      <c r="L75" t="n">
+        <v>143.812791320498</v>
+      </c>
+      <c r="M75" t="n">
+        <v>683858</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-1245.446727</v>
+      </c>
+      <c r="O75" t="n">
+        <v>89.512016083193</v>
+      </c>
+      <c r="P75" t="n">
+        <v>-0.11556</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.132246</v>
+      </c>
+      <c r="R75" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="S75" t="n">
+        <v>-0.002101</v>
+      </c>
+      <c r="T75" t="n">
+        <v>0.01433860038117433</v>
+      </c>
+      <c r="U75" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="V75" t="n">
+        <v>0.009318774988777602</v>
+      </c>
+      <c r="W75" t="n">
+        <v>0.008409307199999999</v>
+      </c>
+      <c r="X75" t="n">
+        <v>-0.043002</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>0.043009</v>
+      </c>
+      <c r="Z75" t="n">
+        <v>-0.001821206635003173</v>
+      </c>
+      <c r="AA75" t="n">
+        <v>-0.002249</v>
+      </c>
+      <c r="AB75" t="n">
+        <v>0.01144083450710502</v>
+      </c>
+      <c r="AC75" t="n">
+        <v>0.0112949502261668</v>
+      </c>
+      <c r="AD75" t="n">
+        <v>0.008215368975723031</v>
+      </c>
+      <c r="AE75" t="n">
+        <v>0.008176539</v>
+      </c>
+      <c r="AF75" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG75" t="n">
+        <v>0.04301580114352299</v>
+      </c>
+      <c r="AH75" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI75" t="n">
+        <v>683858</v>
+      </c>
+      <c r="AJ75" t="n">
+        <v>264076</v>
+      </c>
+      <c r="AK75" t="n">
+        <v>419712</v>
+      </c>
+      <c r="AL75" t="n">
+        <v>12902</v>
+      </c>
+      <c r="AM75" t="n">
+        <v>2734</v>
+      </c>
+      <c r="AN75" t="n">
+        <v>15636</v>
+      </c>
+      <c r="AO75" t="n">
+        <v>0.03989147320286518</v>
+      </c>
+      <c r="AP75" t="n">
+        <v>0.04337597406792291</v>
+      </c>
+      <c r="AQ75" t="n">
+        <v>-0.018882</v>
+      </c>
+      <c r="AR75" t="n">
+        <v>-0.007848000000000001</v>
+      </c>
+      <c r="AS75" t="n">
+        <v>0.003504</v>
+      </c>
+      <c r="AT75" t="n">
+        <v>0.024597</v>
+      </c>
+      <c r="AU75" t="n">
+        <v>0.011352</v>
+      </c>
+      <c r="AV75" t="n">
+        <v>-0.018424</v>
+      </c>
+      <c r="AW75" t="n">
+        <v>-0.007889</v>
+      </c>
+      <c r="AX75" t="n">
+        <v>0.003141</v>
+      </c>
+      <c r="AY75" t="n">
+        <v>0.018931</v>
+      </c>
+      <c r="AZ75" t="n">
+        <v>0.01103</v>
+      </c>
+      <c r="BA75" t="n">
+        <v>-0.0008887905428781375</v>
+      </c>
+      <c r="BB75" t="n">
+        <v>0.01431102764520784</v>
+      </c>
+      <c r="BC75" t="n">
+        <v>238689480875.462</v>
+      </c>
+      <c r="BD75" t="n">
+        <v>5.675151041459209</v>
+      </c>
+      <c r="BE75" t="n">
+        <v>0.1035729672089861</v>
+      </c>
+      <c r="BF75" t="n">
+        <v>-0.09813477944421571</v>
+      </c>
+      <c r="BG75" t="n">
+        <v>0.001960367063261137</v>
+      </c>
+      <c r="BH75" t="n">
+        <v>-0.338411737141495</v>
+      </c>
+      <c r="BI75" t="n">
+        <v>9860681782068.098</v>
+      </c>
+      <c r="BJ75" t="n">
+        <v>1.553251175032938</v>
+      </c>
+      <c r="BK75" t="n">
+        <v>7.219025590519583</v>
+      </c>
+      <c r="BL75" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM75" t="inlineStr">
+        <is>
+          <t>data\0342-0349\python_mov-ref_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BE21">
     <sortState ref="A2:BC25">

</xml_diff>